<commit_message>
trying to get pictures of projects to render
</commit_message>
<xml_diff>
--- a/portfolio/src/Assets/projectsListed.xlsx
+++ b/portfolio/src/Assets/projectsListed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jimij\Documents\GitHub\React_Powered_Portfolio\portfolio\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{88C5280E-E70E-4C2F-BB2E-AEDA49B149C2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F18ADE29-687C-4FF6-A9FD-480D0FC8EEE1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34100" yWindow="930" windowWidth="7150" windowHeight="6860" xr2:uid="{110C090D-0478-4B47-B5AD-1ECCC2F3C05F}"/>
+    <workbookView xWindow="16250" yWindow="7720" windowWidth="19850" windowHeight="15200" xr2:uid="{110C090D-0478-4B47-B5AD-1ECCC2F3C05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -555,7 +555,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D2:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>